<commit_message>
clean + ajout cartouches
</commit_message>
<xml_diff>
--- a/Suivi tache INCA.xlsx
+++ b/Suivi tache INCA.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="124">
   <si>
     <t xml:space="preserve">Tâche</t>
   </si>
@@ -148,13 +148,13 @@
     <t xml:space="preserve">PUBMED : searchAPI.R</t>
   </si>
   <si>
-    <t xml:space="preserve">voir comment enlever ce nombre max. Quel est l'intérêt de cette fonction au final ? VS utiliser directement entrez_search ?</t>
+    <t xml:space="preserve">voir comment enlever ce nombre max. Quel est l'intérêt de cette fonction au final ? VS utiliser directement entrez_search ? + interet keyterm</t>
   </si>
   <si>
     <t xml:space="preserve">PUBMED : fetchAPI.R</t>
   </si>
   <si>
-    <t xml:space="preserve">PUBMED : definition_check_xml.R</t>
+    <t xml:space="preserve">PUBMED : check_xml.R</t>
   </si>
   <si>
     <t xml:space="preserve">PUBMED : full_traitements_xml.R</t>
@@ -175,7 +175,10 @@
     <t xml:space="preserve">TEST : Tests.R</t>
   </si>
   <si>
-    <t xml:space="preserve">plus utilisés ???</t>
+    <t xml:space="preserve">a splitter ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEST : test_integration_all_record.R</t>
   </si>
   <si>
     <t xml:space="preserve">TOOLS : journal.R</t>
@@ -274,6 +277,9 @@
     <t xml:space="preserve">créer une table associant chaque NCT à l'ensemble des publications associées</t>
   </si>
   <si>
+    <t xml:space="preserve">finalement il faudra faire</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gestion des schemas</t>
   </si>
   <si>
@@ -349,6 +355,9 @@
     <t xml:space="preserve">mettre un test à la fin de la remontée postgre</t>
   </si>
   <si>
+    <t xml:space="preserve">a faire dans un temps 2</t>
+  </si>
+  <si>
     <t xml:space="preserve">modifier la fonction split RDS</t>
   </si>
   <si>
@@ -364,16 +373,25 @@
     <t xml:space="preserve">Ecrire le script</t>
   </si>
   <si>
-    <t xml:space="preserve">V1 OK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A améliorer</t>
+    <t xml:space="preserve">V1</t>
   </si>
   <si>
     <t xml:space="preserve">Init de la creation des schema prod/temp/arch</t>
   </si>
   <si>
     <t xml:space="preserve">a integrer dans la partie gestion des schemas ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ça se fait tout seul lors de la gestion des schemas en fait</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il y a des dates qui restent dans mult</t>
+  </si>
+  <si>
+    <t xml:space="preserve">à corriger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ce sont des dates multiples</t>
   </si>
 </sst>
 </file>
@@ -541,15 +559,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D111"/>
+  <dimension ref="A1:D113"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C100" activeCellId="0" sqref="B97:C100"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="70.86"/>
   </cols>
   <sheetData>
@@ -845,126 +863,126 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C36" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="0" t="s">
+      <c r="C36" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C37" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="0" t="s">
+      <c r="C37" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C38" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="0" t="s">
+      <c r="C38" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C39" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="0" t="s">
+      <c r="C39" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C40" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="0" t="s">
+      <c r="C40" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C41" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="0" t="s">
+      <c r="C41" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="0" t="s">
+      <c r="C42" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C43" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="0" t="s">
+      <c r="C43" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C44" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="0" t="s">
+      <c r="C44" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C45" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="0" t="s">
+      <c r="C45" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C46" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="0" t="s">
+      <c r="C46" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C47" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="0" t="s">
+      <c r="C47" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C48" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="0" t="s">
+      <c r="C48" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C49" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="0" t="s">
+      <c r="C49" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C50" s="0" t="s">
+      <c r="C50" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -979,63 +997,63 @@
         <v>42</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="0" t="s">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C52" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="0" t="s">
+      <c r="C52" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C53" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="0" t="s">
+      <c r="C53" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C54" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="0" t="s">
+      <c r="C54" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C55" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="0" t="s">
+      <c r="C55" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C56" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="0" t="s">
+      <c r="C56" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C57" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="0" t="s">
+      <c r="C57" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C58" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C58" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="0" t="s">
         <v>50</v>
       </c>
@@ -1043,51 +1061,51 @@
         <v>51</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="0" t="s">
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C60" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="0" t="s">
+      <c r="C60" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B61" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C61" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="0" t="s">
+      <c r="C61" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B62" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C62" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="0" t="s">
+      <c r="C62" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B63" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C63" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="0" t="s">
+      <c r="C63" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B64" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C64" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="0" t="s">
+      <c r="C64" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B65" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C65" s="0" t="s">
+      <c r="C65" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1195,68 +1213,77 @@
         <v>6</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B79" s="0" t="s">
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B79" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B80" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C79" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="0" t="s">
+      <c r="C80" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B81" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C80" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="B81" s="0" t="s">
+      <c r="C81" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="0" t="s">
+      <c r="B82" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="s">
+      <c r="C82" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B83" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B83" s="0" t="s">
+      <c r="C83" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="0" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="s">
+      <c r="B85" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="B85" s="0" t="s">
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="0" t="s">
+      <c r="B86" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="C86" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="C86" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="1" t="s">
         <v>81</v>
       </c>
@@ -1264,72 +1291,72 @@
         <v>6</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="0" t="s">
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B88" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="C88" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="C88" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="0" t="s">
+      <c r="B89" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="D89" s="0" t="s">
         <v>85</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="B90" s="0" t="s">
+      <c r="B90" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="C90" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
+        <v>88</v>
+      </c>
       <c r="B91" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B93" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="0" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B96" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C96" s="1" t="s">
-        <v>6</v>
+    </row>
+    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B96" s="0" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>6</v>
@@ -1337,7 +1364,7 @@
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>6</v>
@@ -1345,7 +1372,7 @@
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>6</v>
@@ -1353,25 +1380,25 @@
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B101" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="D101" s="0" t="s">
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B101" s="1" t="s">
         <v>99</v>
       </c>
+      <c r="C101" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="0" t="s">
+      <c r="B102" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="B102" s="0" t="s">
+      <c r="D102" s="0" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1383,27 +1410,39 @@
         <v>103</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B104" s="0" t="s">
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B105" s="0" t="s">
+      <c r="B104" s="1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B106" s="0" t="s">
+      <c r="C104" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B105" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="0" t="s">
+      <c r="C105" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B106" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B107" s="0" t="s">
+      <c r="C106" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B107" s="1" t="s">
         <v>108</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1413,35 +1452,63 @@
       <c r="B108" s="0" t="s">
         <v>110</v>
       </c>
+      <c r="D108" s="0" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B110" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="C110" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="D110" s="0" t="s">
+    </row>
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="0" t="s">
+      <c r="B111" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B111" s="0" t="s">
+      <c r="C111" s="1" t="s">
         <v>117</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D112" s="0" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D113" s="0" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>